<commit_message>
22 scenarios done- login page
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/data.xlsx
+++ b/src/test/resources/DataDriven/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Numpy_Ninja_2024\Team2_Selenium_Apr2024\src\test\resources\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A666B0BE-F0CA-4C66-BA5A-82CC8BF0D452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B29FF-13EE-40E4-BC30-7605E146CF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{75B5BE77-69DC-4A61-9AC6-5FC587A3D26F}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>https://lms-frontend-api-hackathon-apr-326235f3973d.herokuapp.com/</t>
   </si>
   <si>
-    <t>https://lms-frontend-api-hackathon-apr-326235f3973d.herokuapp1.com/</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>LMS</t>
+  </si>
+  <si>
+    <t>https://llms-frontend-api-hackathon-apr-326235f3973d.herokuapp.com/</t>
   </si>
 </sst>
 </file>
@@ -123,12 +123,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -469,7 +472,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -489,30 +492,30 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>